<commit_message>
Datos filtrados y exportacion a CSV
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\UNINPAHU\OCTAVO_SEMESTRE\INTELIGENCIA_NEGOCIOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Estudiantes\Documents\Sebas\Upload_Excel_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D49386E-C043-447C-8E00-0FCB40B622E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B46AE6-0A00-4453-9E0A-507AE37A69C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,45 +28,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>CC</t>
   </si>
   <si>
-    <t>Mario Perez</t>
-  </si>
-  <si>
-    <t>Angela Roman</t>
-  </si>
-  <si>
-    <t>TIPO_DOCUMENTO</t>
-  </si>
-  <si>
-    <t>NOMBRES</t>
-  </si>
-  <si>
     <t>SUELDO</t>
   </si>
   <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>SEBAS</t>
-  </si>
-  <si>
-    <t>Cedula</t>
-  </si>
-  <si>
-    <t>Prueba</t>
-  </si>
-  <si>
-    <t>*****</t>
-  </si>
-  <si>
-    <t>Pepito Perez</t>
-  </si>
-  <si>
-    <t>1.1.1.1.1.1</t>
+    <t>TIPO DOCUMENTO</t>
+  </si>
+  <si>
+    <t>NUMERO DOCUMENTO</t>
+  </si>
+  <si>
+    <t>CEDULA</t>
+  </si>
+  <si>
+    <t>CE</t>
   </si>
 </sst>
 </file>
@@ -384,35 +363,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2">
+        <v>1076669247</v>
       </c>
       <c r="C2">
         <v>1500000</v>
@@ -422,8 +402,8 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
+      <c r="B3">
+        <v>1005043696</v>
       </c>
       <c r="C3">
         <v>900000</v>
@@ -431,10 +411,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>74320814</v>
       </c>
       <c r="C4">
         <v>1200000</v>
@@ -442,24 +422,35 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>39743595</v>
+      </c>
+      <c r="C5">
+        <v>-500000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>72257456</v>
+      </c>
+      <c r="C6">
+        <v>344324234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>72257456</v>
+      </c>
+      <c r="C7">
+        <v>458000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>